<commit_message>
added ARA data and highlight option for priority regions
</commit_message>
<xml_diff>
--- a/data/ara.xlsx
+++ b/data/ara.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaeyoungyu/Desktop/Northwestern/Year 4/Quarter 3/STAT 390 - Data Science Project/STAT-390-project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECE84C1-ABBE-FB4F-92F2-0614FD102C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330E746A-B88D-9B4A-8932-B50CE54C6D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="500" windowWidth="28040" windowHeight="15720" xr2:uid="{2B93EBE1-2554-514E-9382-5D84419F350C}"/>
+    <workbookView xWindow="15680" yWindow="500" windowWidth="28040" windowHeight="15720" xr2:uid="{2B93EBE1-2554-514E-9382-5D84419F350C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>community</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>college_enrollment</t>
+  </si>
+  <si>
+    <t>no_internet</t>
   </si>
 </sst>
 </file>
@@ -638,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4EF438-693F-FE45-9D27-7FDAC1C19977}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,7 +666,9 @@
       <c r="D1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -678,6 +683,9 @@
       <c r="D2">
         <v>0.78</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -692,6 +700,9 @@
       <c r="D3">
         <v>0.78</v>
       </c>
+      <c r="E3">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -706,6 +717,9 @@
       <c r="D4">
         <v>0.74</v>
       </c>
+      <c r="E4">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -720,6 +734,9 @@
       <c r="D5">
         <v>0.81</v>
       </c>
+      <c r="E5">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -734,6 +751,9 @@
       <c r="D6">
         <v>0.74</v>
       </c>
+      <c r="E6">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -748,6 +768,9 @@
       <c r="D7">
         <v>0.69</v>
       </c>
+      <c r="E7">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -762,6 +785,9 @@
       <c r="D8">
         <v>0.62</v>
       </c>
+      <c r="E8">
+        <v>0.23</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -776,6 +802,9 @@
       <c r="D9">
         <v>0.73</v>
       </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -790,6 +819,9 @@
       <c r="D10">
         <v>0.72</v>
       </c>
+      <c r="E10">
+        <v>0.12</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -804,6 +836,9 @@
       <c r="D11">
         <v>0.68</v>
       </c>
+      <c r="E11">
+        <v>0.12</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -818,6 +853,9 @@
       <c r="D12">
         <v>0.62</v>
       </c>
+      <c r="E12">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -832,6 +870,9 @@
       <c r="D13">
         <v>0.74</v>
       </c>
+      <c r="E13">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -846,6 +887,9 @@
       <c r="D14">
         <v>0.73</v>
       </c>
+      <c r="E14">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -860,6 +904,9 @@
       <c r="D15">
         <v>0.72</v>
       </c>
+      <c r="E15">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -874,8 +921,11 @@
       <c r="D16">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -888,8 +938,11 @@
       <c r="D17">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -902,8 +955,11 @@
       <c r="D18">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -916,8 +972,11 @@
       <c r="D19">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -930,8 +989,11 @@
       <c r="D20">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -944,8 +1006,11 @@
       <c r="D21">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -958,8 +1023,11 @@
       <c r="D22">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -972,8 +1040,11 @@
       <c r="D23">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -986,8 +1057,11 @@
       <c r="D24">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1000,8 +1074,11 @@
       <c r="D25">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1014,8 +1091,11 @@
       <c r="D26">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1028,8 +1108,11 @@
       <c r="D27">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1042,8 +1125,11 @@
       <c r="D28">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1056,8 +1142,11 @@
       <c r="D29">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1070,8 +1159,11 @@
       <c r="D30">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1084,8 +1176,11 @@
       <c r="D31">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1098,8 +1193,11 @@
       <c r="D32">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1112,8 +1210,11 @@
       <c r="D33">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1126,8 +1227,11 @@
       <c r="D34">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1140,8 +1244,11 @@
       <c r="D35">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1154,8 +1261,11 @@
       <c r="D36">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1168,8 +1278,11 @@
       <c r="D37">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1182,8 +1295,11 @@
       <c r="D38">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1196,8 +1312,11 @@
       <c r="D39">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1210,8 +1329,11 @@
       <c r="D40">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1224,8 +1346,11 @@
       <c r="D41">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1238,8 +1363,11 @@
       <c r="D42">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1252,8 +1380,11 @@
       <c r="D43">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1266,8 +1397,11 @@
       <c r="D44">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1280,8 +1414,11 @@
       <c r="D45">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1294,8 +1431,11 @@
       <c r="D46">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1308,8 +1448,11 @@
       <c r="D47">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1322,8 +1465,11 @@
       <c r="D48">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1336,8 +1482,11 @@
       <c r="D49">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1350,8 +1499,11 @@
       <c r="D50">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1364,8 +1516,11 @@
       <c r="D51">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1378,8 +1533,11 @@
       <c r="D52">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1392,8 +1550,11 @@
       <c r="D53">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1406,8 +1567,11 @@
       <c r="D54">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1420,8 +1584,11 @@
       <c r="D55">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1434,8 +1601,11 @@
       <c r="D56">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1448,8 +1618,11 @@
       <c r="D57">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1462,8 +1635,11 @@
       <c r="D58">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1476,8 +1652,11 @@
       <c r="D59">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1490,8 +1669,11 @@
       <c r="D60">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1504,8 +1686,11 @@
       <c r="D61">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1518,8 +1703,11 @@
       <c r="D62">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1532,8 +1720,11 @@
       <c r="D63">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1546,8 +1737,11 @@
       <c r="D64">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1560,8 +1754,11 @@
       <c r="D65">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1574,8 +1771,11 @@
       <c r="D66">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1588,8 +1788,11 @@
       <c r="D67">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1602,8 +1805,11 @@
       <c r="D68">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1616,8 +1822,11 @@
       <c r="D69">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1630,8 +1839,11 @@
       <c r="D70">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1644,8 +1856,11 @@
       <c r="D71">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1658,8 +1873,11 @@
       <c r="D72">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1672,8 +1890,11 @@
       <c r="D73">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1686,8 +1907,11 @@
       <c r="D74">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1700,8 +1924,11 @@
       <c r="D75">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1714,8 +1941,11 @@
       <c r="D76">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1727,6 +1957,9 @@
       </c>
       <c r="D77">
         <v>0.55000000000000004</v>
+      </c>
+      <c r="E77">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>